<commit_message>
Pushed the updated code
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/UserListDataSet.xlsx
+++ b/src/test/resources/Data/UserListDataSet.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmurugan\eclipse-workspace\MiniProject-1\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C131761-D132-400B-9B5F-472AFCDDF165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D8B026-AA92-4258-ABC5-A0546FB266FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FC5BBF7F-BA56-46ED-941E-6F470CACC640}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FC5BBF7F-BA56-46ED-941E-6F470CACC640}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
     <sheet name="Login_valid_credentials" sheetId="5" r:id="rId2"/>
-    <sheet name="PurchaserDetails" sheetId="6" r:id="rId3"/>
-    <sheet name="Login_Invalid_credentials" sheetId="2" r:id="rId4"/>
-    <sheet name="Menu" sheetId="3" r:id="rId5"/>
-    <sheet name="Categories" sheetId="4" r:id="rId6"/>
+    <sheet name="Login_Invalid_credentials" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -82,79 +79,13 @@
     <t>NotSignUpUser</t>
   </si>
   <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>About us</t>
-  </si>
-  <si>
-    <t>Cart</t>
-  </si>
-  <si>
-    <t>Phones</t>
-  </si>
-  <si>
-    <t>Laptops</t>
-  </si>
-  <si>
-    <t>Monitors</t>
-  </si>
-  <si>
-    <t>Menu1</t>
-  </si>
-  <si>
-    <t>Menu2</t>
-  </si>
-  <si>
-    <t>Menu3</t>
-  </si>
-  <si>
-    <t>Menu4</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
     <t>Welcome chakk27</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>CreditCard</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Chakkaravarthi</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>1234567890123450</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>27</t>
+    <t>chakk35</t>
   </si>
 </sst>
 </file>
@@ -529,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E827C8D-C487-42A6-A9A9-1640CF2DC35C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
@@ -554,10 +485,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -621,10 +552,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -633,65 +564,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485F7DFB-BF04-4019-A4AB-EA8DA8E3B397}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54F84D6-4E83-4A8B-BA83-26D3A93D8582}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -736,83 +608,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA656F85-2C46-4BA7-9F64-95D614E0CF48}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749DA8E6-EF6E-4561-90D9-C138A3BFBEA8}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>